<commit_message>
added correct URLs to Failed_Sources_Corrected_URLs
</commit_message>
<xml_diff>
--- a/data/failed_sources_corrected_urls.xlsx
+++ b/data/failed_sources_corrected_urls.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="19155" windowHeight="8250"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>http://www.mendeley.com/c/5001047982/g/2058663/gomez-2008-land-use-and-west-nile-virus-seroprevalence-in-wild-mammals/</t>
   </si>
@@ -131,13 +131,58 @@
   </si>
   <si>
     <t>Correct URL</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/4974603702/g/2058663/smith-2006-the-vertebrate-fauna-of-ichauway-baker-county-ga/</t>
+  </si>
+  <si>
+    <t>not sure how to find this one</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5076417672/g/2058663/euliss-1996-ecological-studies-at-the-woodworth-study-area-terrestrial-bird-communities-on-the-woodworth-study-area-duplicated-copy-for-dcfs/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5007859122/g/2058663/meyer-1985-classification-of-native-vegetation-at-the-woodworth-station-north-dakota/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5007912492/g/2058663/higgins-1992-waterfowl-production-on-the-woodworth-station-in-south-central-north-dakota--1965-1981/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/4980636152/g/2058663/drew-1998-the-vascular-flora-of-ichauway--baker-county--georgia--a-remnant-longleaf-pine--wiregrass-ecosystem/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5014915452/g/2058663/beckett-1982-forest-vegegation-and-vascular-flora-of-reed-brake-research-natural-area-alabama/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5076426772/g/2058663/euliss-1996-ecological-studies-at-the-woodworth-study-area-upland-vegetation-at-the-woodworth-study-area/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5076428272/g/2058663/euliss-1996-ecological-studies-at-the-woodworth-study-area-effects-of-water-level-changes-on-prairie-pothole-vegetation-structure-and-diversity-in-the-woodworth-study-area--north-dakota-duplicated-copy-for-dcfs/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5009858662/g/2058663/hanson-1989-coleoptera-species-inhabiting-prairie-wetlands-of-the-cottonwood-lake-area-stutsman-county-north-dakota/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5050303512/g/2058663/rice-2010-niche-preference-of-a-coprophagous-scarab-beetle--coleoptera--scarabaeidae--for-summer-moose-dung-in-denali-national-park--alaska/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5017520222/g/2058663/cavey-2004-survey-report-on-the-leaf-beetles-of-cove-point-lng-property-and-vicinity-calvert-county-maryland/</t>
+  </si>
+  <si>
+    <t>could not find</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5018230942/g/2058663/alabama-department-of-conservation-2000-outdoor-alabama-volumes-72-73/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could not find </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +723,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -756,6 +806,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -790,6 +841,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -965,20 +1017,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="114.5703125" customWidth="1"/>
-    <col min="2" max="2" width="89" customWidth="1"/>
+    <col min="1" max="1" width="228.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="251.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="228.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -986,7 +1039,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -994,7 +1047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +1055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1010,7 +1063,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1018,7 +1071,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1026,7 +1079,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1087,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1048,116 +1101,150 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
@@ -1165,11 +1252,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -1177,11 +1266,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
@@ -1189,11 +1280,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
@@ -1201,11 +1294,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1308,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>8</v>
       </c>
@@ -1221,7 +1316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>9</v>
       </c>
@@ -1229,12 +1324,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
correct urls added to failed_sources_corrected_urls
</commit_message>
<xml_diff>
--- a/data/failed_sources_corrected_urls.xlsx
+++ b/data/failed_sources_corrected_urls.xlsx
@@ -136,9 +136,6 @@
     <t>http://www.mendeley.com/c/4974603702/g/2058663/smith-2006-the-vertebrate-fauna-of-ichauway-baker-county-ga/</t>
   </si>
   <si>
-    <t>not sure how to find this one</t>
-  </si>
-  <si>
     <t>http://www.mendeley.com/c/5076417672/g/2058663/euliss-1996-ecological-studies-at-the-woodworth-study-area-terrestrial-bird-communities-on-the-woodworth-study-area-duplicated-copy-for-dcfs/</t>
   </si>
   <si>
@@ -169,13 +166,16 @@
     <t>http://www.mendeley.com/c/5017520222/g/2058663/cavey-2004-survey-report-on-the-leaf-beetles-of-cove-point-lng-property-and-vicinity-calvert-county-maryland/</t>
   </si>
   <si>
-    <t>could not find</t>
-  </si>
-  <si>
     <t>http://www.mendeley.com/c/5018230942/g/2058663/alabama-department-of-conservation-2000-outdoor-alabama-volumes-72-73/</t>
   </si>
   <si>
-    <t xml:space="preserve">could not find </t>
+    <t>http://www.mendeley.com/c/5069088332/g/2058663/mlbsmammalspdf-applicationpdf-object/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/4981987782/g/2058663/usfs-bartlett-experimental-forest/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/c/5069081292/g/2058663/3893285pdf-applicationpdf-object/</t>
   </si>
 </sst>
 </file>
@@ -1020,13 +1020,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="228.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="151.42578125" customWidth="1"/>
     <col min="2" max="2" width="251.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="228.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1117,7 +1117,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1128,7 +1128,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1147,7 +1147,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1155,7 +1155,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -1271,7 +1271,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
added correct url for vectormap to failed_sources_corrected_urls
</commit_message>
<xml_diff>
--- a/data/failed_sources_corrected_urls.xlsx
+++ b/data/failed_sources_corrected_urls.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>http://www.mendeley.com/c/5001047982/g/2058663/gomez-2008-land-use-and-west-nile-virus-seroprevalence-in-wild-mammals/</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>http://www.mendeley.com/c/5069081292/g/2058663/3893285pdf-applicationpdf-object/</t>
+  </si>
+  <si>
+    <t>http://www.mendeley.com/library/showrecent/document/5440490994/#document-5440490994</t>
   </si>
 </sst>
 </file>
@@ -1020,13 +1023,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="151.42578125" customWidth="1"/>
+    <col min="1" max="1" width="154.28515625" customWidth="1"/>
     <col min="2" max="2" width="251.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="228.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1243,7 +1246,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>

</xml_diff>